<commit_message>
Spacing change, and update to table a la implicit math name.
</commit_message>
<xml_diff>
--- a/sbml-level-3/version-1/comp/Table 1.xlsx
+++ b/sbml-level-3/version-1/comp/Table 1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="12015"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="19035" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -91,9 +90,6 @@
     <t>AssignmentRule</t>
   </si>
   <si>
-    <t>Math derived from Reactions</t>
-  </si>
-  <si>
     <t>FunctionDefinition</t>
   </si>
   <si>
@@ -140,6 +136,9 @@
   </si>
   <si>
     <t>&lt;unknown&gt;</t>
+  </si>
+  <si>
+    <t>Implied math for rates of change of species</t>
   </si>
 </sst>
 </file>
@@ -557,7 +556,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="A1:C24"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,7 +579,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" s="15"/>
       <c r="C2" s="8" t="s">
@@ -642,25 +641,25 @@
     </row>
     <row r="8" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="13"/>
       <c r="C8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="8" t="s">
@@ -669,7 +668,7 @@
     </row>
     <row r="11" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="8">
@@ -696,7 +695,7 @@
     </row>
     <row r="14" spans="1:3" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="8" t="s">
@@ -705,7 +704,7 @@
     </row>
     <row r="15" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="8">
@@ -714,7 +713,7 @@
     </row>
     <row r="16" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="8">
@@ -757,10 +756,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -768,15 +767,15 @@
         <v>10</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="8">
@@ -785,16 +784,16 @@
     </row>
     <row r="23" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B24" s="6"/>
       <c r="C24" s="9">

</xml_diff>